<commit_message>
update collect card to 30
</commit_message>
<xml_diff>
--- a/collect_form.xlsx
+++ b/collect_form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eva\Desktop\2023_project\what-does-Shy-say-develop_eva2\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eva\Desktop\2023_project\what-does-Shy-say-develop_eva4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D003776-23FB-407F-A71E-13751B4102DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68DB81A-4B7E-4453-896B-5DF4870C4C7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15096" windowHeight="7416" xr2:uid="{892F6EFF-D678-4179-9C2B-D8069D48D4B1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="19">
   <si>
     <t>no</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -513,11 +513,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CB32BF-1019-4EB4-9C84-5C88AEFA4C74}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -606,6 +604,484 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>